<commit_message>
adding Paper: P2G in future nordic district heating (2017)
</commit_message>
<xml_diff>
--- a/Literatur/Literaturliste.xlsx
+++ b/Literatur/Literaturliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Markus Brandt\OneDrive\Markus\popDH\Literatur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus Brandt\OneDrive\Markus\popDH\Literatur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{D3462C31-A510-4C4E-A6CC-E5B0EB1CE5E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E55BA3C8-2909-48ED-8FBF-46B32FF8EE9C}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="8_{D3462C31-A510-4C4E-A6CC-E5B0EB1CE5E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4BA35290-A953-4427-89FA-5D544C15A918}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="1995" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Literaturliste" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Pos.</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>In ansetzten hat diese Quelle gemacht was ich vorhabe. Aber auch hier wurde wieder die Methanisierung betrachtet.</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -856,10 +859,10 @@
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,7 +1155,9 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="B12" s="10"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>

</xml_diff>